<commit_message>
Update MTH_STS_Majors with 2024 data
</commit_message>
<xml_diff>
--- a/Data/MTH_STS_Majors.xlsx
+++ b/Data/MTH_STS_Majors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rvankrevelen/Dropbox/Elon/Datasets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://elonuniversity-my.sharepoint.com/personal/nbussberg_elon_edu/Documents/Teaching/STS 2300 - 2024-08/Posted/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEB83BF7-5819-E64F-A88D-3D7862389105}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:1_{AEB83BF7-5819-E64F-A88D-3D7862389105}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0347A286-277B-8C4C-8BA0-73004E5F7BAC}"/>
   <bookViews>
-    <workbookView xWindow="21280" yWindow="4300" windowWidth="27240" windowHeight="16440" xr2:uid="{A5581737-E027-B947-813D-22AEECCED70B}"/>
+    <workbookView xWindow="5280" yWindow="500" windowWidth="33120" windowHeight="20000" xr2:uid="{A5581737-E027-B947-813D-22AEECCED70B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -109,9 +109,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -149,7 +149,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -255,7 +255,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -397,7 +397,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -405,15 +405,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E140CCA-909C-4844-A815-96A5481E2A79}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
@@ -442,279 +442,300 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B2">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C2">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D2">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E2">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="F2">
-        <v>2979</v>
+        <v>2956</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="B3">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="C3">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D3">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="E3">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="F3">
-        <v>2967</v>
+        <v>2979</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="B4">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C4">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="D4">
-        <v>34</v>
+        <v>27</v>
+      </c>
+      <c r="E4">
+        <v>11</v>
       </c>
       <c r="F4">
-        <v>2874</v>
+        <v>2964</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="B5">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C5">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D5">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="F5">
-        <v>2888</v>
+        <v>2874</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="B6">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C6">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D6">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F6">
-        <v>2894</v>
+        <v>2888</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="B7">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C7">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D7">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="F7">
-        <v>2848</v>
+        <v>2894</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="B8">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C8">
+        <v>31</v>
+      </c>
+      <c r="D8">
         <v>32</v>
       </c>
-      <c r="D8">
-        <v>37</v>
-      </c>
       <c r="F8">
-        <v>2716</v>
+        <v>2848</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="B9">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="C9">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="D9">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="F9">
-        <v>2610</v>
+        <v>2716</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="B10">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C10">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="D10">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="F10">
-        <v>2563</v>
+        <v>2610</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>2014</v>
+        <v>2015</v>
       </c>
       <c r="B11">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="C11">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D11">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="F11">
-        <v>2639</v>
+        <v>2563</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="B12">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C12">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="D12">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F12">
-        <v>2791</v>
+        <v>2639</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="B13">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C13">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D13">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="F13">
-        <v>2783</v>
+        <v>2791</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="B14">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="C14">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="D14">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F14">
-        <v>2672</v>
+        <v>2783</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>2010</v>
+        <v>2011</v>
       </c>
       <c r="B15">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C15">
-        <v>52</v>
+        <v>63</v>
+      </c>
+      <c r="D15">
+        <v>4</v>
       </c>
       <c r="F15">
-        <v>2472</v>
+        <v>2672</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>2009</v>
+        <v>2010</v>
+      </c>
+      <c r="B16">
+        <v>11</v>
       </c>
       <c r="C16">
-        <v>75</v>
+        <v>52</v>
       </c>
       <c r="F16">
-        <v>2198</v>
+        <v>2472</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>2008</v>
+        <v>2009</v>
       </c>
       <c r="C17">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F17">
-        <v>2182</v>
+        <v>2198</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
+        <v>2008</v>
+      </c>
+      <c r="C18">
+        <v>73</v>
+      </c>
+      <c r="F18">
+        <v>2182</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19">
         <v>2007</v>
       </c>
-      <c r="C18">
+      <c r="C19">
         <v>54</v>
       </c>
-      <c r="F18">
+      <c r="F19">
         <v>2105</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>